<commit_message>
removing history from list
</commit_message>
<xml_diff>
--- a/data/Israel/covid19-data-israel.xlsx
+++ b/data/Israel/covid19-data-israel.xlsx
@@ -422,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1385,7 +1385,7 @@
         <v>2444</v>
       </c>
       <c r="C42" s="4">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42" s="4">
         <v>16</v>
@@ -1408,7 +1408,7 @@
         <v>2782</v>
       </c>
       <c r="C43" s="4">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D43" s="4">
         <v>19</v>
@@ -1431,7 +1431,7 @@
         <v>3204</v>
       </c>
       <c r="C44" s="4">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D44" s="4">
         <v>26</v>
@@ -1454,7 +1454,7 @@
         <v>3723</v>
       </c>
       <c r="C45" s="4">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D45" s="4">
         <v>40</v>
@@ -1477,7 +1477,7 @@
         <v>4244</v>
       </c>
       <c r="C46" s="4">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D46" s="4">
         <v>59</v>
@@ -1500,7 +1500,7 @@
         <v>4647</v>
       </c>
       <c r="C47" s="4">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D47" s="4">
         <v>81</v>
@@ -1523,7 +1523,7 @@
         <v>5254</v>
       </c>
       <c r="C48" s="4">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D48" s="4">
         <v>103</v>
@@ -1546,7 +1546,7 @@
         <v>5950</v>
       </c>
       <c r="C49" s="4">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D49" s="4">
         <v>123</v>
@@ -1569,7 +1569,7 @@
         <v>6563</v>
       </c>
       <c r="C50" s="4">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D50" s="4">
         <v>162</v>
@@ -1592,7 +1592,7 @@
         <v>7747</v>
       </c>
       <c r="C51" s="4">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D51" s="4">
         <v>201</v>
@@ -1615,7 +1615,7 @@
         <v>9092</v>
       </c>
       <c r="C52" s="4">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D52" s="4">
         <v>221</v>
@@ -1638,7 +1638,7 @@
         <v>10748</v>
       </c>
       <c r="C53" s="4">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D53" s="4">
         <v>257</v>
@@ -1661,7 +1661,7 @@
         <v>12866</v>
       </c>
       <c r="C54" s="4">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D54" s="4">
         <v>306</v>
@@ -1684,7 +1684,7 @@
         <v>14947</v>
       </c>
       <c r="C55" s="4">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D55" s="4">
         <v>295</v>
@@ -1707,7 +1707,7 @@
         <v>17272</v>
       </c>
       <c r="C56" s="4">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D56" s="4">
         <v>287</v>
@@ -1730,7 +1730,7 @@
         <v>19369</v>
       </c>
       <c r="C57" s="4">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D57" s="4">
         <v>276</v>
@@ -1753,7 +1753,7 @@
         <v>22705</v>
       </c>
       <c r="C58" s="4">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="D58" s="4">
         <v>323</v>
@@ -1776,7 +1776,7 @@
         <v>26329</v>
       </c>
       <c r="C59" s="4">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="D59" s="4">
         <v>350</v>
@@ -1799,7 +1799,7 @@
         <v>31110</v>
       </c>
       <c r="C60" s="4">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="D60" s="4">
         <v>393</v>
@@ -1822,7 +1822,7 @@
         <v>37033</v>
       </c>
       <c r="C61" s="4">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="D61" s="4">
         <v>412</v>
@@ -1845,7 +1845,7 @@
         <v>43542</v>
       </c>
       <c r="C62" s="4">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="D62" s="4">
         <v>464</v>
@@ -1868,7 +1868,7 @@
         <v>49287</v>
       </c>
       <c r="C63" s="4">
-        <v>3426</v>
+        <v>3425</v>
       </c>
       <c r="D63" s="4">
         <v>515</v>
@@ -1891,7 +1891,7 @@
         <v>54997</v>
       </c>
       <c r="C64" s="4">
-        <v>3906</v>
+        <v>3905</v>
       </c>
       <c r="D64" s="4">
         <v>512</v>
@@ -1914,7 +1914,7 @@
         <v>62561</v>
       </c>
       <c r="C65" s="4">
-        <v>4438</v>
+        <v>4437</v>
       </c>
       <c r="D65" s="4">
         <v>541</v>
@@ -1937,7 +1937,7 @@
         <v>69652</v>
       </c>
       <c r="C66" s="4">
-        <v>4984</v>
+        <v>4983</v>
       </c>
       <c r="D66" s="4">
         <v>617</v>
@@ -1960,7 +1960,7 @@
         <v>77612</v>
       </c>
       <c r="C67" s="4">
-        <v>5713</v>
+        <v>5712</v>
       </c>
       <c r="D67" s="4">
         <v>665</v>
@@ -1983,7 +1983,7 @@
         <v>86593</v>
       </c>
       <c r="C68" s="4">
-        <v>6408</v>
+        <v>6407</v>
       </c>
       <c r="D68" s="4">
         <v>767</v>
@@ -2006,7 +2006,7 @@
         <v>96809</v>
       </c>
       <c r="C69" s="4">
-        <v>7127</v>
+        <v>7126</v>
       </c>
       <c r="D69" s="4">
         <v>810</v>
@@ -2029,7 +2029,7 @@
         <v>107133</v>
       </c>
       <c r="C70" s="4">
-        <v>7726</v>
+        <v>7725</v>
       </c>
       <c r="D70" s="4">
         <v>799</v>
@@ -2052,7 +2052,7 @@
         <v>113649</v>
       </c>
       <c r="C71" s="4">
-        <v>8154</v>
+        <v>8153</v>
       </c>
       <c r="D71" s="4">
         <v>785</v>
@@ -2075,7 +2075,7 @@
         <v>123089</v>
       </c>
       <c r="C72" s="4">
-        <v>8733</v>
+        <v>8732</v>
       </c>
       <c r="D72" s="4">
         <v>822</v>
@@ -2095,10 +2095,10 @@
         <v>43927</v>
       </c>
       <c r="B73" s="4">
-        <v>130587</v>
+        <v>130586</v>
       </c>
       <c r="C73" s="4">
-        <v>9185</v>
+        <v>9184</v>
       </c>
       <c r="D73" s="4">
         <v>804</v>
@@ -2118,10 +2118,10 @@
         <v>43928</v>
       </c>
       <c r="B74" s="4">
-        <v>137514</v>
+        <v>137513</v>
       </c>
       <c r="C74" s="4">
-        <v>9564</v>
+        <v>9563</v>
       </c>
       <c r="D74" s="4">
         <v>743</v>
@@ -2141,10 +2141,10 @@
         <v>43929</v>
       </c>
       <c r="B75" s="4">
-        <v>143383</v>
+        <v>143382</v>
       </c>
       <c r="C75" s="4">
-        <v>9902</v>
+        <v>9901</v>
       </c>
       <c r="D75" s="4">
         <v>689</v>
@@ -2164,10 +2164,10 @@
         <v>43930</v>
       </c>
       <c r="B76" s="4">
-        <v>149131</v>
+        <v>149130</v>
       </c>
       <c r="C76" s="4">
-        <v>10247</v>
+        <v>10246</v>
       </c>
       <c r="D76" s="4">
         <v>662</v>
@@ -2187,10 +2187,10 @@
         <v>43931</v>
       </c>
       <c r="B77" s="4">
-        <v>156458</v>
+        <v>156457</v>
       </c>
       <c r="C77" s="4">
-        <v>10608</v>
+        <v>10607</v>
       </c>
       <c r="D77" s="4">
         <v>664</v>
@@ -2210,10 +2210,10 @@
         <v>43932</v>
       </c>
       <c r="B78" s="4">
-        <v>163150</v>
+        <v>163149</v>
       </c>
       <c r="C78" s="4">
-        <v>10953</v>
+        <v>10952</v>
       </c>
       <c r="D78" s="4">
         <v>620</v>
@@ -2233,10 +2233,10 @@
         <v>43933</v>
       </c>
       <c r="B79" s="4">
-        <v>173770</v>
+        <v>173769</v>
       </c>
       <c r="C79" s="4">
-        <v>11511</v>
+        <v>11510</v>
       </c>
       <c r="D79" s="4">
         <v>661</v>
@@ -2256,10 +2256,10 @@
         <v>43934</v>
       </c>
       <c r="B80" s="4">
-        <v>184729</v>
+        <v>184728</v>
       </c>
       <c r="C80" s="4">
-        <v>11955</v>
+        <v>11954</v>
       </c>
       <c r="D80" s="4">
         <v>681</v>
@@ -2279,10 +2279,10 @@
         <v>43935</v>
       </c>
       <c r="B81" s="4">
-        <v>197392</v>
+        <v>197391</v>
       </c>
       <c r="C81" s="4">
-        <v>12362</v>
+        <v>12361</v>
       </c>
       <c r="D81" s="4">
         <v>669</v>
@@ -2302,10 +2302,10 @@
         <v>43936</v>
       </c>
       <c r="B82" s="4">
-        <v>206842</v>
+        <v>206841</v>
       </c>
       <c r="C82" s="4">
-        <v>12674</v>
+        <v>12673</v>
       </c>
       <c r="D82" s="4">
         <v>666</v>
@@ -2325,19 +2325,19 @@
         <v>43937</v>
       </c>
       <c r="B83" s="4">
-        <v>219622</v>
+        <v>219624</v>
       </c>
       <c r="C83" s="4">
-        <v>12976</v>
+        <v>12975</v>
       </c>
       <c r="D83" s="4">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="E83" s="4">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F83" s="4">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G83" s="4">
         <v>143</v>
@@ -2348,19 +2348,19 @@
         <v>43938</v>
       </c>
       <c r="B84" s="4">
-        <v>231187</v>
+        <v>231189</v>
       </c>
       <c r="C84" s="4">
-        <v>13278</v>
+        <v>13277</v>
       </c>
       <c r="D84" s="4">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="E84" s="4">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F84" s="4">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G84" s="4">
         <v>152</v>
@@ -2371,19 +2371,19 @@
         <v>43939</v>
       </c>
       <c r="B85" s="4">
-        <v>241818</v>
+        <v>241820</v>
       </c>
       <c r="C85" s="4">
-        <v>13589</v>
+        <v>13588</v>
       </c>
       <c r="D85" s="4">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E85" s="4">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F85" s="4">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G85" s="4">
         <v>163</v>
@@ -2394,19 +2394,19 @@
         <v>43940</v>
       </c>
       <c r="B86" s="4">
-        <v>253103</v>
+        <v>253106</v>
       </c>
       <c r="C86" s="4">
-        <v>13878</v>
+        <v>13877</v>
       </c>
       <c r="D86" s="4">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E86" s="4">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F86" s="4">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G86" s="4">
         <v>171</v>
@@ -2417,19 +2417,19 @@
         <v>43941</v>
       </c>
       <c r="B87" s="4">
-        <v>268241</v>
+        <v>268245</v>
       </c>
       <c r="C87" s="4">
-        <v>14181</v>
+        <v>14180</v>
       </c>
       <c r="D87" s="4">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="E87" s="4">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F87" s="4">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G87" s="4">
         <v>177</v>
@@ -2440,19 +2440,19 @@
         <v>43942</v>
       </c>
       <c r="B88" s="4">
-        <v>281731</v>
+        <v>281733</v>
       </c>
       <c r="C88" s="4">
-        <v>14474</v>
+        <v>14473</v>
       </c>
       <c r="D88" s="4">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="E88" s="4">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F88" s="4">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G88" s="4">
         <v>186</v>
@@ -2466,19 +2466,42 @@
         <v>295030</v>
       </c>
       <c r="C89" s="4">
-        <v>14704</v>
+        <v>14703</v>
       </c>
       <c r="D89" s="4">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="E89" s="4">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F89" s="4">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G89" s="4">
         <v>189</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="3">
+        <v>43944</v>
+      </c>
+      <c r="B90" s="4">
+        <v>309188</v>
+      </c>
+      <c r="C90" s="4">
+        <v>14985</v>
+      </c>
+      <c r="D90" s="4">
+        <v>484</v>
+      </c>
+      <c r="E90" s="4">
+        <v>140</v>
+      </c>
+      <c r="F90" s="4">
+        <v>110</v>
+      </c>
+      <c r="G90" s="4">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>